<commit_message>
SXL 1.1: Update for compatibility
- Convert "timestamp" to "string", because it doesn't officially exist in 3.2
- Remove any trailing _list because it is only used for comma separated values
  during schema validation
</commit_message>
<xml_diff>
--- a/YAML/SXL-example.xlsx
+++ b/YAML/SXL-example.xlsx
@@ -13378,10 +13378,10 @@
         <v>minToGEstimate</v>
       </c>
       <c r="F31" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G31" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H31" s="17" t="str">
         <v xml:space="preserve">Time stamp for the minimum time for the signal group to go to green. If the signal group is green, it is the minimum time for the next green.
@@ -13391,10 +13391,10 @@
         <v>maxToGEstimate</v>
       </c>
       <c r="J31" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="K31" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="L31" s="17" t="str">
         <v xml:space="preserve">Time stamp for the maximum time for the signal group to go to green. If the signal group is green, it is the maximum time for the next green.
@@ -13404,10 +13404,10 @@
         <v>likelyToGEstimate</v>
       </c>
       <c r="N31" s="21" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="O31" s="21" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="P31" s="21" t="str">
         <v xml:space="preserve">Time stamp for the most likely time for the signal group to go to green. If the signal group is green, it is the most likely time for the next green.
@@ -13429,10 +13429,10 @@
         <v>minToREstimate</v>
       </c>
       <c r="V31" s="21" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="W31" s="21" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="X31" s="21" t="str">
         <v xml:space="preserve">Time stamp for the minimum time for the signal group to go to red. If the signal group is red, it is the minimum time for the next red.
@@ -13442,10 +13442,10 @@
         <v>maxToREstimate</v>
       </c>
       <c r="Z31" s="21" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="AA31" s="21" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="AB31" s="21" t="str">
         <v xml:space="preserve">Time stamp for the maximum time for the signal group to go to red. If the signal group is red, it is the maximum time for the next red.
@@ -13455,10 +13455,10 @@
         <v>likelyToREstimate</v>
       </c>
       <c r="AD31" s="21" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="AE31" s="21" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="AF31" s="21" t="str">
         <v xml:space="preserve">Time stamp for the most likely time for the signal group to go to red. If the signal group is red, it is the most likely time for the next red.
@@ -13801,7 +13801,7 @@
   type: string
   description: ID of the priority request
 t:
-  type: timestamp
+  type: string
   description: |-
     Timestamp, indicating when the priority last changed state.
     Format according to W3C XML dateTime with a resolution of 3 decimal places.
@@ -14103,10 +14103,10 @@
         <v>timestamp</v>
       </c>
       <c r="J45" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="K45" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="L45" s="17" t="str">
         <v>Time stamp of the checksum. Format according to W3C XML dateTime with a resolution of 3 decimal places. All time stamps in UTC. E.g. 2009-10-02T14:34:34.341Z</v>
@@ -14156,10 +14156,10 @@
         <v>timestamp</v>
       </c>
       <c r="J46" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="K46" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="L46" s="17" t="str">
         <v>Time stamp of the config. Format according to W3C XML dateTime with a resolution of 3 decimal places. All time stamps in UTC. E.g. 2009-10-02T14:34:34.341Z</v>
@@ -14194,10 +14194,10 @@
         <v>starttime</v>
       </c>
       <c r="F47" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G47" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H47" s="17" t="str">
         <v>Time stamp for start of measuring. Format according to W3C XML dateTime with a resolution of 3 decimal places. All time stamps in UTC. E.g. 2009-10-02T14:34:34.341Z</v>
@@ -14231,10 +14231,10 @@
         <v>starttime</v>
       </c>
       <c r="F48" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G48" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H48" s="17" t="str">
         <v xml:space="preserve">Time stamp for start of measuring. Format according to W3C
@@ -14270,10 +14270,10 @@
         <v>starttime</v>
       </c>
       <c r="F49" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G49" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H49" s="17" t="str">
         <v xml:space="preserve">Time stamp for start of measuring. Format according to W3C
@@ -14309,10 +14309,10 @@
         <v>starttime</v>
       </c>
       <c r="F50" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G50" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H50" s="17" t="str">
         <v xml:space="preserve">Time stamp for start of measuring. Format according to W3C
@@ -14444,10 +14444,10 @@
         <v>start</v>
       </c>
       <c r="F51" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G51" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H51" s="17" t="str">
         <v>Time stamp for start of measuring. Format according to W3C XML dateTime with a resolution of 3 decimal places. All time stamps in UTC. E.g. 2009-10-02T14:34:34.341Z</v>
@@ -14484,10 +14484,10 @@
         <v>start</v>
       </c>
       <c r="F52" s="17" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G52" s="17" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H52" s="17" t="str">
         <v xml:space="preserve">Time stamp for start of measuring. Format according to W3C
@@ -14525,10 +14525,10 @@
         <v>start</v>
       </c>
       <c r="F53" s="21" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G53" s="21" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H53" s="21" t="str">
         <v xml:space="preserve">Time stamp for start of measuring. Format according to W3C
@@ -14566,10 +14566,10 @@
         <v>start</v>
       </c>
       <c r="F54" s="21" t="str">
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="G54" s="21" t="str">
-        <v/>
+        <v>[string]</v>
       </c>
       <c r="H54" s="21" t="str">
         <v xml:space="preserve">Time stamp for start of measuring. Format according to W3C

</xml_diff>